<commit_message>
Updated progress and added data disdtribution file
</commit_message>
<xml_diff>
--- a/dataDistributions.xlsx
+++ b/dataDistributions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\EECS4414\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B860DC-CE2C-4B05-8859-1987E5AFFEDE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F82CB5-EF34-4E60-A1E1-BDF77AA55C5D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14220" windowHeight="7875" xr2:uid="{3713A4BA-2265-4026-88C9-9799802B4F26}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14220" windowHeight="7875" activeTab="2" xr2:uid="{3713A4BA-2265-4026-88C9-9799802B4F26}"/>
   </bookViews>
   <sheets>
     <sheet name="Out" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="195">
   <si>
     <t xml:space="preserve">Afghanistan </t>
   </si>
@@ -6866,7 +6866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD9584D-305A-4940-A939-F2186ECFDC46}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+    <sheetView topLeftCell="A172" workbookViewId="0">
       <selection activeCell="P193" sqref="P193"/>
     </sheetView>
   </sheetViews>
@@ -9970,10 +9970,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3145FF89-B1EF-417C-A008-503AFC764035}">
-  <dimension ref="A1:B190"/>
+  <dimension ref="A1:B192"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11501,6 +11501,15 @@
         <v>0.70491523495278097</v>
       </c>
     </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>194</v>
+      </c>
+      <c r="B192">
+        <f>AVERAGE(B2:B190)</f>
+        <v>0.85759749719883438</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:B190">
     <sortCondition descending="1" ref="B2:B190"/>

</xml_diff>